<commit_message>
added time course and explicit selection graphs
</commit_message>
<xml_diff>
--- a/analysis/data/participant-log-connectives-cog-control.xlsx
+++ b/analysis/data/participant-log-connectives-cog-control.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/m2-thesis/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/m2-thesis/connectives_cog_control/analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E38ACAD-D2D5-FB46-A4E3-5C852A4092F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13819A80-0203-EF4A-9847-EF698902C34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="500" windowWidth="21180" windowHeight="16020" xr2:uid="{A94A81EA-A6A8-8A46-9CBF-41F27DE3F102}"/>
+    <workbookView xWindow="-360" yWindow="500" windowWidth="21180" windowHeight="16020" xr2:uid="{A94A81EA-A6A8-8A46-9CBF-41F27DE3F102}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="220">
   <si>
     <t>participant_number</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>child</t>
+  </si>
+  <si>
+    <t>21032301</t>
   </si>
 </sst>
 </file>
@@ -1073,9 +1076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F4D11E-DF6D-7544-BC30-EB23F7D74275}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1721,8 +1724,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>21032301</v>
+      <c r="A16" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>39</v>
@@ -4951,7 +4954,7 @@
         <v>40</v>
       </c>
       <c r="M92" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
@@ -5077,7 +5080,7 @@
         <v>40</v>
       </c>
       <c r="M95" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added data files for participants who stopped partway through, updated analysis
</commit_message>
<xml_diff>
--- a/analysis/data/participant-log-connectives-cog-control.xlsx
+++ b/analysis/data/participant-log-connectives-cog-control.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/m2-thesis/connectives_cog_control/analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/m2-thesis/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13819A80-0203-EF4A-9847-EF698902C34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33726C4B-AE8B-E849-9AC5-1B861646E33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="500" windowWidth="21180" windowHeight="16020" xr2:uid="{A94A81EA-A6A8-8A46-9CBF-41F27DE3F102}"/>
+    <workbookView xWindow="3740" yWindow="500" windowWidth="21180" windowHeight="16020" xr2:uid="{A94A81EA-A6A8-8A46-9CBF-41F27DE3F102}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="223">
   <si>
     <t>participant_number</t>
   </si>
@@ -696,6 +696,15 @@
   </si>
   <si>
     <t>21032301</t>
+  </si>
+  <si>
+    <t>31032302</t>
+  </si>
+  <si>
+    <t>20032302</t>
+  </si>
+  <si>
+    <t>30032305</t>
   </si>
 </sst>
 </file>
@@ -744,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -758,6 +767,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1076,9 +1088,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F4D11E-DF6D-7544-BC30-EB23F7D74275}">
   <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M96" sqref="M96"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M80" sqref="M80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1346,7 +1358,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="7">
         <v>20032301</v>
       </c>
       <c r="B7" s="4">
@@ -1388,8 +1400,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>20032302</v>
+      <c r="A8" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="B8" s="4">
         <v>20032302</v>
@@ -1426,7 +1438,7 @@
         <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1598,7 +1610,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="7">
         <v>20032308</v>
       </c>
       <c r="B13" s="4">
@@ -1636,7 +1648,7 @@
         <v>38</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1727,8 +1739,8 @@
       <c r="A16" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>39</v>
+      <c r="B16" s="4">
+        <v>2103230301</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>218</v>
@@ -1753,13 +1765,13 @@
         <v>7</v>
       </c>
       <c r="J16" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K16" t="s">
         <v>64</v>
       </c>
       <c r="L16" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="M16" t="s">
         <v>67</v>
@@ -1812,7 +1824,7 @@
         <v>21032303</v>
       </c>
       <c r="B18" s="4">
-        <v>2103230301</v>
+        <v>210323022</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>218</v>
@@ -1888,7 +1900,7 @@
         <v>40</v>
       </c>
       <c r="M19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -2308,7 +2320,7 @@
         <v>62</v>
       </c>
       <c r="M29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -2690,8 +2702,8 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>30032305</v>
+      <c r="A39" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="B39" s="5">
         <v>30032386</v>
@@ -3026,8 +3038,8 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>31032302</v>
+      <c r="A47" s="7" t="s">
+        <v>220</v>
       </c>
       <c r="B47" s="4">
         <v>30032356</v>
@@ -3404,7 +3416,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3530,7 +3542,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -4408,7 +4420,7 @@
         <v>141</v>
       </c>
       <c r="M79" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
@@ -4870,7 +4882,7 @@
         <v>40</v>
       </c>
       <c r="M90" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
@@ -4912,7 +4924,7 @@
         <v>40</v>
       </c>
       <c r="M91" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>